<commit_message>
Test Excel Design Durchlauf 2
</commit_message>
<xml_diff>
--- a/documents/project management/Test/Durchlauf 2/Abnahmetest_Go Happy_Design.xlsx
+++ b/documents/project management/Test/Durchlauf 2/Abnahmetest_Go Happy_Design.xlsx
@@ -1,15 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="5" rupBuild="4505"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28760" windowHeight="16560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="24240" windowHeight="13740" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Design" sheetId="4" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="124519" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="74" uniqueCount="70">
   <si>
     <t>ID</t>
   </si>
@@ -66,12 +66,6 @@
     <t>Dem Anwender wird eine Liste von Bars zur Verfügung gestellt, die durchsucht werden kann und eine Auswahl getroffen werden kann.</t>
   </si>
   <si>
-    <t>Ergebnis Backend</t>
-  </si>
-  <si>
-    <t>Kommentar Backend</t>
-  </si>
-  <si>
     <t>Abnahmetest durch das Team "Frontend"</t>
   </si>
   <si>
@@ -211,13 +205,37 @@
   </si>
   <si>
     <t>Es erscheint ein Pop Up fenster in welches man einen Text zur Fehlermeldung ientragen kann. Dieser kann anschließend abgeschickt oder aber auch verworfen werden. Es folgt eine Bestätigung.</t>
+  </si>
+  <si>
+    <t>Ergebnis Design</t>
+  </si>
+  <si>
+    <t>Kommentar Design</t>
+  </si>
+  <si>
+    <t>Es wird mir jeden Wochentag diegleiche Route angezeigt.</t>
+  </si>
+  <si>
+    <t>Es wird nur die Freitagsroute angezeigt.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Umlaute können (teilw.) nicht richtig angezeigt werden. Bsp: beim Sausalitos "Jumbo Cocktail f??r 5???" </t>
+  </si>
+  <si>
+    <t>Über Button "kopieren" wird Link nicht in Zwischenspeicher kopiert. Manuelles kopieren des Llinks aus dem Textfeld ist möglich.</t>
+  </si>
+  <si>
+    <t>Ich konnte den Fehlerfall nicht nachstellen.</t>
+  </si>
+  <si>
+    <t>Ergebnis wird morgen nachgetragen</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="7" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="7">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -552,159 +570,159 @@
     </xf>
   </cellXfs>
   <cellStyles count="153">
-    <cellStyle name="Besuchter Link" xfId="2" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="4" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="6" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="8" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="10" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="12" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="14" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="16" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="18" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="20" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="22" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="24" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="26" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="28" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="30" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="32" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="34" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="36" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="38" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="40" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="42" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="44" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="46" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="48" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="50" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="52" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="54" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="56" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="58" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="60" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="62" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="64" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="66" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="68" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="70" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="72" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="74" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="76" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="78" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="80" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="82" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="84" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="86" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="88" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="90" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="92" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="94" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="96" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="98" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="100" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="102" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="104" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="106" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="108" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="110" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="112" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="114" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="116" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="118" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="120" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="122" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="124" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="126" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="128" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="130" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="132" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="134" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="136" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="138" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="140" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="142" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="144" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="146" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="148" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="150" builtinId="9" hidden="1"/>
-    <cellStyle name="Besuchter Link" xfId="152" builtinId="9" hidden="1"/>
-    <cellStyle name="Link" xfId="1" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="3" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="5" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="7" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="9" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="11" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="13" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="15" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="17" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="19" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="21" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="23" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="25" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="27" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="29" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="31" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="33" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="35" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="37" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="39" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="41" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="43" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="45" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="47" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="49" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="51" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="53" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="55" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="57" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="59" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="61" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="63" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="65" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="67" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="69" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="71" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="73" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="75" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="77" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="79" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="81" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="83" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="85" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="87" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="89" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="91" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="93" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="95" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="97" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="99" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="101" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="103" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="105" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="107" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="109" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="111" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="113" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="115" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="117" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="119" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="121" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="123" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="125" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="127" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="129" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="131" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="133" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="135" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="137" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="139" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="141" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="143" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="145" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="147" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="149" builtinId="8" hidden="1"/>
-    <cellStyle name="Link" xfId="151" builtinId="8" hidden="1"/>
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="8" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="54" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="76" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="78" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="80" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="82" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="84" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="86" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="88" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="90" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="92" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="94" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="96" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="98" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="100" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="102" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="104" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="106" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="108" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="110" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="112" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="114" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="116" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="118" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="120" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="122" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="124" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="126" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="128" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="130" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="132" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="134" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="136" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="138" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="140" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="142" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="144" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="146" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="148" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="150" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="152" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="7" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="53" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="75" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="77" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="79" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="81" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="83" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="85" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="87" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="89" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="91" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="93" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="95" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="97" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="99" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="101" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="103" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="105" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="107" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="109" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="111" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="113" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="115" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="117" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="119" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="121" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="123" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="125" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="127" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="129" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="131" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="133" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="135" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="137" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="139" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="141" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="143" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="145" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="147" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="149" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="151" builtinId="8" hidden="1"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
@@ -724,7 +742,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -755,7 +773,7 @@
         <scheme val="minor"/>
       </font>
       <numFmt numFmtId="0" formatCode="General"/>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -791,7 +809,7 @@
           <bgColor rgb="FFDCE6F1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -827,7 +845,7 @@
           <bgColor rgb="FFDCE6F1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right/>
@@ -863,7 +881,7 @@
           <bgColor rgb="FFDCE6F1"/>
         </patternFill>
       </fill>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" relativeIndent="255" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color rgb="FF95B3D7"/>
@@ -934,8 +952,8 @@
     <tableColumn id="1" name="ID" dataDxfId="4"/>
     <tableColumn id="2" name="Testszenario" dataDxfId="3"/>
     <tableColumn id="3" name="Erwartungen" dataDxfId="2"/>
-    <tableColumn id="4" name="Ergebnis Backend" dataDxfId="1"/>
-    <tableColumn id="5" name="Kommentar Backend" dataDxfId="0"/>
+    <tableColumn id="4" name="Ergebnis Design" dataDxfId="1"/>
+    <tableColumn id="5" name="Kommentar Design" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight9" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1262,25 +1280,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
     <col min="1" max="1" width="6.5" customWidth="1"/>
     <col min="2" max="2" width="63" customWidth="1"/>
-    <col min="3" max="3" width="74.6640625" customWidth="1"/>
+    <col min="3" max="3" width="74.625" customWidth="1"/>
     <col min="4" max="4" width="18.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="21.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:5">
@@ -1294,13 +1312,13 @@
         <v>1</v>
       </c>
       <c r="D2" s="7" t="s">
-        <v>15</v>
+        <v>62</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="30">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="31.5">
       <c r="A3" s="8">
         <v>1</v>
       </c>
@@ -1308,194 +1326,232 @@
         <v>2</v>
       </c>
       <c r="C3" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="D3" s="2"/>
+        <v>36</v>
+      </c>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
       <c r="E3" s="11"/>
     </row>
-    <row r="4" spans="1:5" ht="45">
+    <row r="4" spans="1:5" ht="47.25">
       <c r="A4" s="10">
         <v>2</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C4" s="16" t="s">
         <v>8</v>
       </c>
       <c r="D4" s="4"/>
-      <c r="E4" s="12"/>
-    </row>
-    <row r="5" spans="1:5" ht="60">
+      <c r="E4" s="12" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" ht="63">
       <c r="A5" s="8">
         <v>3</v>
       </c>
       <c r="B5" s="9" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="C5" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D5" s="2"/>
+      <c r="D5" s="2">
+        <v>1</v>
+      </c>
       <c r="E5" s="11"/>
     </row>
-    <row r="6" spans="1:5" ht="60">
+    <row r="6" spans="1:5" ht="63">
       <c r="A6" s="10">
         <v>4</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D6" s="3"/>
-      <c r="E6" s="13"/>
-    </row>
-    <row r="7" spans="1:5" ht="60">
+      <c r="D6" s="3">
+        <v>0</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" ht="63">
       <c r="A7" s="8">
         <v>5</v>
       </c>
       <c r="B7" s="9" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C7" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D7" s="2"/>
+      <c r="D7" s="2">
+        <v>1</v>
+      </c>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" ht="60">
+    <row r="8" spans="1:5" ht="63">
       <c r="A8" s="10">
         <v>6</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="3"/>
+      <c r="D8" s="3">
+        <v>1</v>
+      </c>
       <c r="E8" s="14"/>
     </row>
-    <row r="9" spans="1:5" ht="60">
+    <row r="9" spans="1:5" ht="63">
       <c r="A9" s="8">
         <v>7</v>
       </c>
       <c r="B9" s="9" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C9" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="D9" s="5"/>
+      <c r="D9" s="5">
+        <v>1</v>
+      </c>
       <c r="E9" s="5"/>
     </row>
-    <row r="10" spans="1:5" ht="30">
+    <row r="10" spans="1:5" ht="31.5">
       <c r="A10" s="10">
         <v>8</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="C10" s="1" t="s">
-        <v>39</v>
-      </c>
-      <c r="D10" s="3"/>
+        <v>37</v>
+      </c>
+      <c r="D10" s="3">
+        <v>1</v>
+      </c>
       <c r="E10" s="3"/>
     </row>
-    <row r="11" spans="1:5" ht="30">
+    <row r="11" spans="1:5" ht="31.5">
       <c r="A11" s="8">
         <v>9</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C11" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-    </row>
-    <row r="12" spans="1:5" ht="30">
+      <c r="D11" s="5">
+        <v>1</v>
+      </c>
+      <c r="E11" s="15"/>
+    </row>
+    <row r="12" spans="1:5" ht="31.5">
       <c r="A12" s="10">
         <v>10</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C12" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="D12" s="4"/>
+        <v>39</v>
+      </c>
+      <c r="D12" s="4">
+        <v>1</v>
+      </c>
       <c r="E12" s="4"/>
     </row>
-    <row r="13" spans="1:5">
+    <row r="13" spans="1:5" ht="31.5">
       <c r="A13" s="8">
         <v>11</v>
       </c>
       <c r="B13" s="9" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C13" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
-    </row>
-    <row r="14" spans="1:5" ht="30">
+      <c r="D13" s="2">
+        <v>0</v>
+      </c>
+      <c r="E13" s="11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" ht="31.5">
       <c r="A14" s="10">
         <v>12</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="3"/>
+      <c r="D14" s="3">
+        <v>1</v>
+      </c>
       <c r="E14" s="3"/>
     </row>
-    <row r="15" spans="1:5" ht="30">
+    <row r="15" spans="1:5" ht="78.75">
       <c r="A15" s="8">
         <v>13</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C15" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-    </row>
-    <row r="16" spans="1:5" ht="30">
+      <c r="D15" s="2">
+        <v>0</v>
+      </c>
+      <c r="E15" s="11" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" ht="31.5">
       <c r="A16" s="10">
         <v>14</v>
       </c>
       <c r="B16" s="1" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>42</v>
-      </c>
-      <c r="D16" s="4"/>
+        <v>40</v>
+      </c>
+      <c r="D16" s="4">
+        <v>1</v>
+      </c>
       <c r="E16" s="4"/>
     </row>
-    <row r="17" spans="1:5" ht="30">
+    <row r="17" spans="1:5" ht="110.25">
       <c r="A17" s="8">
         <v>15</v>
       </c>
       <c r="B17" s="9" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C17" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-    </row>
-    <row r="18" spans="1:5" ht="30">
+      <c r="D17" s="5">
+        <v>0</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" ht="31.5">
       <c r="A18" s="10">
         <v>16</v>
       </c>
@@ -1503,103 +1559,119 @@
         <v>5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>43</v>
-      </c>
-      <c r="D18" s="3"/>
+        <v>41</v>
+      </c>
+      <c r="D18" s="3">
+        <v>1</v>
+      </c>
       <c r="E18" s="3"/>
     </row>
-    <row r="19" spans="1:5" ht="45">
+    <row r="19" spans="1:5" ht="47.25">
       <c r="A19" s="8">
         <v>17</v>
       </c>
       <c r="B19" s="9" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="C19" s="9" t="s">
-        <v>18</v>
-      </c>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-    </row>
-    <row r="20" spans="1:5" ht="45">
+        <v>16</v>
+      </c>
+      <c r="D19" s="2">
+        <v>1</v>
+      </c>
+      <c r="E19" s="11"/>
+    </row>
+    <row r="20" spans="1:5" ht="47.25">
       <c r="A20" s="10">
         <v>18</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D20" s="3"/>
+        <v>42</v>
+      </c>
+      <c r="D20" s="3">
+        <v>1</v>
+      </c>
       <c r="E20" s="3"/>
     </row>
-    <row r="21" spans="1:5" ht="30">
+    <row r="21" spans="1:5" ht="31.5">
       <c r="A21" s="8">
         <v>19</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C21" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="D21" s="5"/>
+        <v>43</v>
+      </c>
+      <c r="D21" s="5">
+        <v>1</v>
+      </c>
       <c r="E21" s="5"/>
     </row>
-    <row r="22" spans="1:5" ht="45">
+    <row r="22" spans="1:5" ht="47.25">
       <c r="A22" s="10">
         <v>20</v>
       </c>
       <c r="B22" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D22" s="3"/>
+        <v>44</v>
+      </c>
+      <c r="D22" s="3">
+        <v>1</v>
+      </c>
       <c r="E22" s="3"/>
     </row>
-    <row r="23" spans="1:5" ht="45">
+    <row r="23" spans="1:5" ht="47.25">
       <c r="A23" s="8">
         <v>21</v>
       </c>
       <c r="B23" s="9" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C23" s="9" t="s">
-        <v>47</v>
-      </c>
-      <c r="D23" s="2"/>
+        <v>45</v>
+      </c>
+      <c r="D23" s="2">
+        <v>1</v>
+      </c>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="45">
+    <row r="24" spans="1:5" ht="47.25">
       <c r="A24" s="10">
         <v>22</v>
       </c>
       <c r="B24" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C24" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D24" s="4"/>
+      <c r="D24" s="4">
+        <v>1</v>
+      </c>
       <c r="E24" s="4"/>
     </row>
-    <row r="25" spans="1:5" ht="30">
+    <row r="25" spans="1:5" ht="31.5">
       <c r="A25" s="8">
         <v>23</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C25" s="9" t="s">
-        <v>48</v>
-      </c>
-      <c r="D25" s="2"/>
+        <v>46</v>
+      </c>
+      <c r="D25" s="2">
+        <v>1</v>
+      </c>
       <c r="E25" s="11"/>
     </row>
-    <row r="26" spans="1:5" ht="30">
+    <row r="26" spans="1:5" ht="31.5">
       <c r="A26" s="10">
         <v>24</v>
       </c>
@@ -1609,99 +1681,115 @@
       <c r="C26" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="D26" s="3"/>
+      <c r="D26" s="3">
+        <v>1</v>
+      </c>
       <c r="E26" s="3"/>
     </row>
-    <row r="27" spans="1:5" ht="45">
+    <row r="27" spans="1:5" ht="47.25">
       <c r="A27" s="8">
         <v>25</v>
       </c>
       <c r="B27" s="9" t="s">
+        <v>59</v>
+      </c>
+      <c r="C27" s="9" t="s">
         <v>61</v>
       </c>
-      <c r="C27" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="2"/>
+      <c r="D27" s="2">
+        <v>1</v>
+      </c>
       <c r="E27" s="11"/>
     </row>
-    <row r="28" spans="1:5" ht="30">
+    <row r="28" spans="1:5" ht="31.5">
       <c r="A28" s="10">
         <v>26</v>
       </c>
       <c r="B28" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="D28" s="3"/>
+        <v>47</v>
+      </c>
+      <c r="D28" s="3">
+        <v>1</v>
+      </c>
       <c r="E28" s="13"/>
     </row>
-    <row r="29" spans="1:5" ht="45">
+    <row r="29" spans="1:5" ht="47.25">
       <c r="A29" s="8">
         <v>27</v>
       </c>
       <c r="B29" s="9" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="C29" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="D29" s="5"/>
+        <v>48</v>
+      </c>
+      <c r="D29" s="5">
+        <v>1</v>
+      </c>
       <c r="E29" s="15"/>
     </row>
-    <row r="30" spans="1:5" ht="30">
+    <row r="30" spans="1:5" ht="31.5">
       <c r="A30" s="10">
         <v>28</v>
       </c>
       <c r="B30" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C30" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D30" s="4"/>
+        <v>49</v>
+      </c>
+      <c r="D30" s="4">
+        <v>1</v>
+      </c>
       <c r="E30" s="4"/>
     </row>
-    <row r="31" spans="1:5" ht="30">
+    <row r="31" spans="1:5" ht="31.5">
       <c r="A31" s="8">
         <v>29</v>
       </c>
       <c r="B31" s="9" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="C31" s="9" t="s">
-        <v>52</v>
-      </c>
-      <c r="D31" s="5"/>
+        <v>50</v>
+      </c>
+      <c r="D31" s="5">
+        <v>1</v>
+      </c>
       <c r="E31" s="5"/>
     </row>
-    <row r="32" spans="1:5" ht="30">
+    <row r="32" spans="1:5" ht="31.5">
       <c r="A32" s="10">
         <v>30</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C32" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="D32" s="4"/>
+        <v>51</v>
+      </c>
+      <c r="D32" s="4">
+        <v>1</v>
+      </c>
       <c r="E32" s="4"/>
     </row>
-    <row r="33" spans="1:5">
+    <row r="33" spans="1:5" ht="31.5">
       <c r="A33" s="8">
         <v>31</v>
       </c>
       <c r="B33" s="9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C33" s="9" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D33" s="5"/>
-      <c r="E33" s="5"/>
+      <c r="E33" s="15" t="s">
+        <v>69</v>
+      </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="D3:D33">

</xml_diff>